<commit_message>
adicionado comprovante de pagamento
</commit_message>
<xml_diff>
--- a/planilhas/resultado.xlsx
+++ b/planilhas/resultado.xlsx
@@ -17,29 +17,6 @@
     </ext>
   </extLst>
 </workbook>
-</file>
-
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
-  <si>
-    <t xml:space="preserve">03</t>
-  </si>
-  <si>
-    <t xml:space="preserve">13</t>
-  </si>
-  <si>
-    <t xml:space="preserve">27</t>
-  </si>
-  <si>
-    <t xml:space="preserve">55</t>
-  </si>
-  <si>
-    <t xml:space="preserve">56</t>
-  </si>
-  <si>
-    <t xml:space="preserve">59</t>
-  </si>
-</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -244,38 +221,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="F4" activeCellId="0" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="1" style="1" width="11.53"/>
   </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-  </sheetData>
+  <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>